<commit_message>
Added option to speed up and down
Still not working very well….
</commit_message>
<xml_diff>
--- a/Remotes codes.xlsx
+++ b/Remotes codes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
   <si>
     <t>apagado</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>IRLIB</t>
+  </si>
+  <si>
+    <t>40BFCA35</t>
   </si>
 </sst>
 </file>
@@ -250,8 +253,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -271,15 +298,39 @@
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -612,7 +663,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -956,7 +1007,7 @@
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>37</v>

</xml_diff>